<commit_message>
Update SSC INVIGILATORS NEW 2023.xlsx
</commit_message>
<xml_diff>
--- a/INVIGILATIONS 2022-23/SSC/SSC INVIGILATORS NEW 2023.xlsx
+++ b/INVIGILATIONS 2022-23/SSC/SSC INVIGILATORS NEW 2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\docs\INVIGILATIONS 2022-23\SSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EA3181-9252-4410-8CDD-A672F15F5C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8555A759-F7E4-4D7C-B859-AA37C55B784D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -384,7 +384,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +419,33 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -513,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,24 +570,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -587,15 +596,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -937,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V220"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="E97" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M103" sqref="M103"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A41" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J100" sqref="J100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,14 +994,14 @@
     <col min="3" max="3" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26" style="22" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="22"/>
-    <col min="15" max="15" width="14.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" style="32" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5703125" style="32" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="31" customWidth="1"/>
+    <col min="13" max="13" width="26" style="16" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="16"/>
+    <col min="15" max="15" width="14.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
@@ -964,44 +1010,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="H1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="18"/>
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="H1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="12"/>
     </row>
     <row r="2" spans="1:22" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="H2" s="12" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="H2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="26"/>
       <c r="J2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="27"/>
       <c r="L2" s="27"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
     </row>
     <row r="3" spans="1:22" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1019,24 +1065,24 @@
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
       <c r="Q3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1075,24 +1121,21 @@
       <c r="F4" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="29">
         <v>1</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="16">
-        <v>9490751700</v>
-      </c>
-      <c r="M4" s="24"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="I4" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="29">
+        <v>8555063978</v>
+      </c>
       <c r="Q4" t="s">
         <v>54</v>
       </c>
@@ -1100,7 +1143,7 @@
         <v>103</v>
       </c>
       <c r="S4" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q4,DATA,2,FALSE),"")</f>
+        <f t="shared" ref="S4:S46" si="0">IFERROR(VLOOKUP(Q4,DATA,2,FALSE),"")</f>
         <v>BOYS</v>
       </c>
       <c r="T4" s="8" t="b">
@@ -1133,24 +1176,21 @@
       <c r="F5" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="29">
         <v>2</v>
       </c>
-      <c r="I5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="16">
-        <v>9492096504</v>
-      </c>
-      <c r="M5" s="24"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="I5" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="29">
+        <v>9398199012</v>
+      </c>
       <c r="Q5" t="s">
         <v>55</v>
       </c>
@@ -1158,11 +1198,11 @@
         <v>103</v>
       </c>
       <c r="S5" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q5,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T5" s="8" t="b">
-        <f t="shared" ref="T5:T46" si="0">EXACT(R5,S5)</f>
+        <f t="shared" ref="T5:T46" si="1">EXACT(R5,S5)</f>
         <v>1</v>
       </c>
       <c r="U5" t="s">
@@ -1191,19 +1231,19 @@
       <c r="F6" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="29">
         <v>3</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="7" t="s">
+      <c r="J6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="29">
         <v>9490948936</v>
       </c>
       <c r="M6" s="10"/>
@@ -1216,11 +1256,11 @@
         <v>103</v>
       </c>
       <c r="S6" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q6,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T6" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U6" t="s">
@@ -1249,24 +1289,21 @@
       <c r="F7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="29">
         <v>4</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L7" s="6">
-        <v>8500286206</v>
-      </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
+      <c r="I7" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="29">
+        <v>9494144304</v>
+      </c>
       <c r="Q7" t="s">
         <v>57</v>
       </c>
@@ -1274,11 +1311,11 @@
         <v>103</v>
       </c>
       <c r="S7" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q7,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T7" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U7" t="s">
@@ -1307,24 +1344,21 @@
       <c r="F8" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="29">
         <v>5</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="6">
-        <v>9492994288</v>
-      </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
+      <c r="I8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="29">
+        <v>8500470262</v>
+      </c>
       <c r="Q8" t="s">
         <v>58</v>
       </c>
@@ -1332,11 +1366,11 @@
         <v>103</v>
       </c>
       <c r="S8" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q8,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T8" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U8" t="s">
@@ -1365,24 +1399,21 @@
       <c r="F9" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="29">
         <v>6</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="6">
-        <v>8985912623</v>
-      </c>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
+      <c r="I9" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="29">
+        <v>9441020561</v>
+      </c>
       <c r="Q9" t="s">
         <v>59</v>
       </c>
@@ -1390,11 +1421,11 @@
         <v>103</v>
       </c>
       <c r="S9" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q9,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T9" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U9" t="s">
@@ -1423,19 +1454,19 @@
       <c r="F10" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="29">
         <v>7</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="7" t="s">
+      <c r="J10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="29">
         <v>9494328436</v>
       </c>
       <c r="M10" s="10"/>
@@ -1448,11 +1479,11 @@
         <v>103</v>
       </c>
       <c r="S10" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q10,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T10" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U10" t="s">
@@ -1481,19 +1512,19 @@
       <c r="F11" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="29">
         <v>8</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="7" t="s">
+      <c r="J11" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="29">
         <v>9492090842</v>
       </c>
       <c r="Q11" t="s">
@@ -1503,11 +1534,11 @@
         <v>103</v>
       </c>
       <c r="S11" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q11,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T11" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U11" t="s">
@@ -1525,13 +1556,13 @@
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="6"/>
-      <c r="H12" s="6">
+      <c r="H12" s="29">
         <v>9</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="6"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="29"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -1542,11 +1573,11 @@
         <v>103</v>
       </c>
       <c r="S12" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q12,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T12" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U12" t="s">
@@ -1564,13 +1595,13 @@
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
       <c r="E13" s="6"/>
-      <c r="H13" s="6">
+      <c r="H13" s="29">
         <v>10</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="6"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="29"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1581,11 +1612,11 @@
         <v>103</v>
       </c>
       <c r="S13" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q13,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>ZPHS</v>
       </c>
       <c r="T13" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U13" t="s">
@@ -1603,13 +1634,13 @@
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
-      <c r="H14" s="6">
+      <c r="H14" s="29">
         <v>11</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="6"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="29"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -1620,11 +1651,11 @@
         <v>103</v>
       </c>
       <c r="S14" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q14,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>PTG</v>
       </c>
       <c r="T14" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U14" t="s">
@@ -1642,13 +1673,13 @@
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" s="6"/>
-      <c r="H15" s="6">
-        <v>12</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="6"/>
+      <c r="H15" s="29">
+        <v>12</v>
+      </c>
+      <c r="I15" s="30"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="29"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -1659,11 +1690,11 @@
         <v>104</v>
       </c>
       <c r="S15" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q15,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>ZPHS</v>
       </c>
       <c r="T15" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U15" t="s">
@@ -1682,11 +1713,11 @@
         <v>104</v>
       </c>
       <c r="S16" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q16,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T16" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U16" t="s">
@@ -1705,11 +1736,11 @@
         <v>104</v>
       </c>
       <c r="S17" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q17,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>ZPHS</v>
       </c>
       <c r="T17" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U17" t="s">
@@ -1728,11 +1759,11 @@
         <v>104</v>
       </c>
       <c r="S18" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q18,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>ZPHS</v>
       </c>
       <c r="T18" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U18" t="s">
@@ -1751,11 +1782,11 @@
         <v>104</v>
       </c>
       <c r="S19" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q19,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>ZPHS</v>
       </c>
       <c r="T19" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U19" t="s">
@@ -1774,11 +1805,11 @@
         <v>104</v>
       </c>
       <c r="S20" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q20,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T20" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U20" t="s">
@@ -1797,11 +1828,11 @@
         <v>104</v>
       </c>
       <c r="S21" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q21,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T21" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U21" t="s">
@@ -1820,11 +1851,11 @@
         <v>104</v>
       </c>
       <c r="S22" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q22,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T22" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U22" t="s">
@@ -1843,11 +1874,11 @@
         <v>104</v>
       </c>
       <c r="S23" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q23,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T23" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U23" t="s">
@@ -1866,11 +1897,11 @@
         <v>108</v>
       </c>
       <c r="S24" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q24,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>TKB</v>
       </c>
       <c r="T24" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U24" t="s">
@@ -1889,11 +1920,11 @@
         <v>108</v>
       </c>
       <c r="S25" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q25,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>TKB</v>
       </c>
       <c r="T25" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U25" t="s">
@@ -1904,22 +1935,22 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="A26" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
       <c r="F26" s="8"/>
-      <c r="H26" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="18"/>
+      <c r="H26" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="12"/>
       <c r="Q26" t="s">
         <v>79</v>
       </c>
@@ -1927,11 +1958,11 @@
         <v>108</v>
       </c>
       <c r="S26" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q26,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>TKB</v>
       </c>
       <c r="T26" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U26" t="s">
@@ -1942,26 +1973,26 @@
       </c>
     </row>
     <row r="27" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="22"/>
+      <c r="C27" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
       <c r="F27" s="8"/>
-      <c r="H27" s="12" t="s">
+      <c r="H27" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="12"/>
+      <c r="I27" s="26"/>
       <c r="J27" s="27" t="s">
         <v>52</v>
       </c>
       <c r="K27" s="27"/>
       <c r="L27" s="27"/>
-      <c r="M27" s="19"/>
+      <c r="M27" s="13"/>
       <c r="Q27" t="s">
         <v>80</v>
       </c>
@@ -1969,11 +2000,11 @@
         <v>108</v>
       </c>
       <c r="S27" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q27,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>TKB</v>
       </c>
       <c r="T27" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U27" t="s">
@@ -2000,22 +2031,22 @@
         <v>5</v>
       </c>
       <c r="F28" s="8"/>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="K28" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="L28" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M28" s="20"/>
+      <c r="M28" s="14"/>
       <c r="Q28" t="s">
         <v>81</v>
       </c>
@@ -2023,11 +2054,11 @@
         <v>108</v>
       </c>
       <c r="S28" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q28,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="T28" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U28" t="s">
@@ -2056,22 +2087,22 @@
       <c r="F29" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="29">
         <v>1</v>
       </c>
-      <c r="I29" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="L29" s="16">
-        <v>8555063978</v>
-      </c>
-      <c r="M29" s="24"/>
+      <c r="I29" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="29">
+        <v>9490751700</v>
+      </c>
+      <c r="M29" s="18"/>
       <c r="Q29" t="s">
         <v>82</v>
       </c>
@@ -2079,11 +2110,11 @@
         <v>108</v>
       </c>
       <c r="S29" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q29,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="T29" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U29" t="s">
@@ -2112,22 +2143,22 @@
       <c r="F30" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="29">
         <v>2</v>
       </c>
-      <c r="I30" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="L30" s="16">
-        <v>9398199012</v>
-      </c>
-      <c r="M30" s="24"/>
+      <c r="I30" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="29">
+        <v>9492096504</v>
+      </c>
+      <c r="M30" s="18"/>
       <c r="Q30" t="s">
         <v>83</v>
       </c>
@@ -2135,11 +2166,11 @@
         <v>108</v>
       </c>
       <c r="S30" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q30,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>TKB</v>
       </c>
       <c r="T30" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U30" t="s">
@@ -2168,19 +2199,19 @@
       <c r="F31" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="29">
         <v>3</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J31" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="L31" s="6">
+      <c r="L31" s="29">
         <v>6303871088</v>
       </c>
       <c r="M31" s="10"/>
@@ -2191,11 +2222,11 @@
         <v>108</v>
       </c>
       <c r="S31" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q31,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T31" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U31" t="s">
@@ -2224,19 +2255,19 @@
       <c r="F32" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="29">
         <v>4</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I32" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="7" t="s">
+      <c r="J32" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L32" s="6">
+      <c r="L32" s="29">
         <v>9494083460</v>
       </c>
       <c r="M32" s="10"/>
@@ -2247,11 +2278,11 @@
         <v>108</v>
       </c>
       <c r="S32" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q32,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="T32" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U32" t="s">
@@ -2280,19 +2311,19 @@
       <c r="F33" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="29">
         <v>5</v>
       </c>
-      <c r="I33" s="7" t="s">
+      <c r="I33" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="J33" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="7" t="s">
+      <c r="J33" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="L33" s="6">
+      <c r="L33" s="29">
         <v>9494329193</v>
       </c>
       <c r="M33" s="10"/>
@@ -2303,11 +2334,11 @@
         <v>105</v>
       </c>
       <c r="S33" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q33,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T33" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U33" t="s">
@@ -2336,19 +2367,19 @@
       <c r="F34" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="29">
         <v>6</v>
       </c>
-      <c r="I34" s="7" t="s">
+      <c r="I34" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="J34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K34" s="7" t="s">
+      <c r="J34" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="L34" s="6">
+      <c r="L34" s="29">
         <v>7989979188</v>
       </c>
       <c r="M34" s="10"/>
@@ -2359,11 +2390,11 @@
         <v>105</v>
       </c>
       <c r="S34" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q34,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T34" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U34" t="s">
@@ -2392,19 +2423,19 @@
       <c r="F35" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="29">
         <v>7</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I35" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" s="7" t="s">
+      <c r="J35" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="L35" s="6">
+      <c r="L35" s="29">
         <v>9492019120</v>
       </c>
       <c r="M35" s="10"/>
@@ -2415,11 +2446,11 @@
         <v>105</v>
       </c>
       <c r="S35" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q35,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T35" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U35" t="s">
@@ -2448,20 +2479,20 @@
       <c r="F36" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36" s="29">
         <v>8</v>
       </c>
-      <c r="I36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K36" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L36" s="6">
-        <v>9441020561</v>
+      <c r="I36" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J36" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L36" s="29">
+        <v>8985912623</v>
       </c>
       <c r="Q36" t="s">
         <v>43</v>
@@ -2470,11 +2501,11 @@
         <v>105</v>
       </c>
       <c r="S36" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q36,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T36" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U36" t="s">
@@ -2503,20 +2534,20 @@
       <c r="F37" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="29">
         <v>9</v>
       </c>
-      <c r="I37" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="L37" s="6">
-        <v>9494144304</v>
+      <c r="I37" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="L37" s="29">
+        <v>8500286206</v>
       </c>
       <c r="Q37" t="s">
         <v>44</v>
@@ -2525,11 +2556,11 @@
         <v>105</v>
       </c>
       <c r="S37" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q37,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T37" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U37" t="s">
@@ -2558,20 +2589,20 @@
       <c r="F38" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="29">
         <v>10</v>
       </c>
-      <c r="I38" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L38" s="6">
-        <v>8500470262</v>
+      <c r="I38" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J38" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" s="29">
+        <v>9492994288</v>
       </c>
       <c r="Q38" t="s">
         <v>45</v>
@@ -2580,11 +2611,11 @@
         <v>105</v>
       </c>
       <c r="S38" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q38,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T38" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U38" t="s">
@@ -2613,20 +2644,20 @@
       <c r="F39" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="29">
         <v>11</v>
       </c>
-      <c r="I39" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L39" s="6">
-        <v>6305961181</v>
+      <c r="I39" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="J39" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="29">
+        <v>9494779417</v>
       </c>
       <c r="Q39" s="8" t="s">
         <v>8</v>
@@ -2635,11 +2666,11 @@
         <v>102</v>
       </c>
       <c r="S39" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q39,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>ZPHS</v>
       </c>
       <c r="T39" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U39" s="8" t="s">
@@ -2658,13 +2689,13 @@
       <c r="D40" s="7"/>
       <c r="E40" s="6"/>
       <c r="F40" s="8"/>
-      <c r="H40" s="6">
-        <v>12</v>
-      </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="6"/>
+      <c r="H40" s="29">
+        <v>12</v>
+      </c>
+      <c r="I40" s="30"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="29"/>
       <c r="M40" s="10"/>
       <c r="Q40" s="8" t="s">
         <v>11</v>
@@ -2673,11 +2704,11 @@
         <v>102</v>
       </c>
       <c r="S40" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q40,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T40" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U40" s="8" t="s">
@@ -2694,11 +2725,11 @@
       <c r="D41" s="10"/>
       <c r="E41" s="9"/>
       <c r="F41" s="8"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="9"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="33"/>
       <c r="M41" s="10"/>
       <c r="Q41" s="8" t="s">
         <v>14</v>
@@ -2707,11 +2738,11 @@
         <v>102</v>
       </c>
       <c r="S41" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q41,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T41" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U41" s="8" t="s">
@@ -2728,11 +2759,11 @@
       <c r="D42" s="10"/>
       <c r="E42" s="9"/>
       <c r="F42" s="8"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="9"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="33"/>
       <c r="M42" s="10"/>
       <c r="Q42" s="8" t="s">
         <v>16</v>
@@ -2741,11 +2772,11 @@
         <v>102</v>
       </c>
       <c r="S42" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q42,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>ZPHS</v>
       </c>
       <c r="T42" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U42" s="8" t="s">
@@ -2762,11 +2793,11 @@
       <c r="D43" s="10"/>
       <c r="E43" s="9"/>
       <c r="F43" s="8"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="9"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="33"/>
       <c r="M43" s="10"/>
       <c r="Q43" s="8" t="s">
         <v>18</v>
@@ -2775,11 +2806,11 @@
         <v>102</v>
       </c>
       <c r="S43" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q43,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T43" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U43" s="8" t="s">
@@ -2796,11 +2827,11 @@
       <c r="D44" s="10"/>
       <c r="E44" s="9"/>
       <c r="F44" s="8"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="9"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="33"/>
       <c r="M44" s="10"/>
       <c r="Q44" s="8" t="s">
         <v>20</v>
@@ -2809,11 +2840,11 @@
         <v>102</v>
       </c>
       <c r="S44" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q44,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>BOYS</v>
       </c>
       <c r="T44" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U44" s="8" t="s">
@@ -2830,11 +2861,11 @@
       <c r="D45" s="10"/>
       <c r="E45" s="9"/>
       <c r="F45" s="8"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="9"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="33"/>
       <c r="M45" s="10"/>
       <c r="Q45" s="8" t="s">
         <v>22</v>
@@ -2843,11 +2874,11 @@
         <v>102</v>
       </c>
       <c r="S45" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q45,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T45" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U45" s="8" t="s">
@@ -2864,11 +2895,11 @@
       <c r="D46" s="10"/>
       <c r="E46" s="9"/>
       <c r="F46" s="8"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="9"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="33"/>
       <c r="M46" s="10"/>
       <c r="Q46" s="8" t="s">
         <v>24</v>
@@ -2877,11 +2908,11 @@
         <v>102</v>
       </c>
       <c r="S46" s="8" t="str">
-        <f>IFERROR(VLOOKUP(Q46,DATA,2,FALSE),"")</f>
+        <f t="shared" si="0"/>
         <v>REG</v>
       </c>
       <c r="T46" s="8" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U46" s="8" t="s">
@@ -2898,11 +2929,11 @@
       <c r="D47" s="10"/>
       <c r="E47" s="9"/>
       <c r="F47" s="8"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="9"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="33"/>
       <c r="M47" s="10"/>
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
@@ -2934,44 +2965,44 @@
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:22" ht="21" x14ac:dyDescent="0.35">
-      <c r="A52" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
+      <c r="A52" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
       <c r="F52" s="8"/>
-      <c r="H52" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="18"/>
+      <c r="H52" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="12"/>
     </row>
     <row r="53" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="13" t="s">
+      <c r="B53" s="22"/>
+      <c r="C53" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
       <c r="F53" s="8"/>
-      <c r="H53" s="12" t="s">
+      <c r="H53" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I53" s="12"/>
+      <c r="I53" s="26"/>
       <c r="J53" s="27" t="s">
         <v>53</v>
       </c>
       <c r="K53" s="27"/>
       <c r="L53" s="27"/>
-      <c r="M53" s="19"/>
+      <c r="M53" s="13"/>
     </row>
     <row r="54" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
@@ -2990,22 +3021,22 @@
         <v>5</v>
       </c>
       <c r="F54" s="8"/>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I54" s="5" t="s">
+      <c r="I54" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J54" s="5" t="s">
+      <c r="J54" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K54" s="5" t="s">
+      <c r="K54" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L54" s="5" t="s">
+      <c r="L54" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M54" s="20"/>
+      <c r="M54" s="14"/>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
@@ -3026,24 +3057,24 @@
       <c r="F55" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G55" s="17"/>
-      <c r="H55" s="6">
+      <c r="G55" s="11"/>
+      <c r="H55" s="29">
         <v>1</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I55" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="J55" s="6" t="s">
+      <c r="J55" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="K55" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="L55" s="6">
+      <c r="L55" s="29">
         <v>9492621203</v>
       </c>
       <c r="M55" s="10"/>
-      <c r="N55" s="25"/>
+      <c r="N55" s="19"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
@@ -3064,24 +3095,24 @@
       <c r="F56" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G56" s="17"/>
-      <c r="H56" s="6">
+      <c r="G56" s="11"/>
+      <c r="H56" s="29">
         <v>2</v>
       </c>
-      <c r="I56" s="7" t="s">
+      <c r="I56" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="J56" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K56" s="7" t="s">
+      <c r="J56" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K56" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="L56" s="6">
+      <c r="L56" s="29">
         <v>9490302874</v>
       </c>
       <c r="M56" s="10"/>
-      <c r="N56" s="25"/>
+      <c r="N56" s="19"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
@@ -3102,24 +3133,24 @@
       <c r="F57" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="6">
+      <c r="G57" s="11"/>
+      <c r="H57" s="29">
         <v>3</v>
       </c>
-      <c r="I57" s="7" t="s">
+      <c r="I57" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="J57" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K57" s="7" t="s">
+      <c r="J57" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K57" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="L57" s="6">
+      <c r="L57" s="29">
         <v>8985169260</v>
       </c>
       <c r="M57" s="10"/>
-      <c r="N57" s="25"/>
+      <c r="N57" s="19"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
@@ -3140,24 +3171,24 @@
       <c r="F58" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G58" s="17"/>
-      <c r="H58" s="6">
+      <c r="G58" s="11"/>
+      <c r="H58" s="29">
         <v>4</v>
       </c>
-      <c r="I58" s="7" t="s">
+      <c r="I58" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="J58" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K58" s="7" t="s">
+      <c r="J58" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K58" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="L58" s="6">
+      <c r="L58" s="29">
         <v>7382157706</v>
       </c>
       <c r="M58" s="10"/>
-      <c r="N58" s="25"/>
+      <c r="N58" s="19"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
@@ -3178,24 +3209,24 @@
       <c r="F59" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="6">
+      <c r="G59" s="11"/>
+      <c r="H59" s="29">
         <v>5</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I59" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="J59" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K59" s="7" t="s">
+      <c r="J59" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K59" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="L59" s="6">
+      <c r="L59" s="29">
         <v>9440266236</v>
       </c>
       <c r="M59" s="10"/>
-      <c r="N59" s="25"/>
+      <c r="N59" s="19"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
@@ -3216,24 +3247,24 @@
       <c r="F60" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G60" s="17"/>
-      <c r="H60" s="6">
+      <c r="G60" s="11"/>
+      <c r="H60" s="29">
         <v>6</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I60" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J60" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K60" s="7" t="s">
+      <c r="J60" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K60" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="L60" s="6">
+      <c r="L60" s="29">
         <v>9491842195</v>
       </c>
       <c r="M60" s="10"/>
-      <c r="N60" s="25"/>
+      <c r="N60" s="19"/>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
@@ -3254,24 +3285,24 @@
       <c r="F61" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="6">
+      <c r="G61" s="11"/>
+      <c r="H61" s="29">
         <v>7</v>
       </c>
-      <c r="I61" s="7" t="s">
+      <c r="I61" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="J61" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K61" s="7" t="s">
+      <c r="J61" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K61" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L61" s="6">
+      <c r="L61" s="29">
         <v>9491570619</v>
       </c>
       <c r="M61" s="10"/>
-      <c r="N61" s="25"/>
+      <c r="N61" s="19"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
@@ -3292,24 +3323,24 @@
       <c r="F62" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="6">
+      <c r="G62" s="11"/>
+      <c r="H62" s="29">
         <v>8</v>
       </c>
-      <c r="I62" s="7" t="s">
+      <c r="I62" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="J62" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K62" s="7" t="s">
+      <c r="J62" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K62" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="L62" s="6">
+      <c r="L62" s="29">
         <v>9494325704</v>
       </c>
       <c r="M62" s="10"/>
-      <c r="N62" s="25"/>
+      <c r="N62" s="19"/>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
@@ -3330,24 +3361,24 @@
       <c r="F63" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="6">
+      <c r="G63" s="11"/>
+      <c r="H63" s="29">
         <v>9</v>
       </c>
-      <c r="I63" s="7" t="s">
+      <c r="I63" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="J63" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K63" s="7" t="s">
+      <c r="J63" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K63" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="L63" s="6">
+      <c r="L63" s="29">
         <v>8500249423</v>
       </c>
       <c r="M63" s="10"/>
-      <c r="N63" s="25"/>
+      <c r="N63" s="19"/>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
@@ -3358,13 +3389,13 @@
       <c r="D64" s="7"/>
       <c r="E64" s="6"/>
       <c r="F64" s="8"/>
-      <c r="H64" s="6">
+      <c r="H64" s="29">
         <v>10</v>
       </c>
-      <c r="I64" s="7"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="6"/>
+      <c r="I64" s="30"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="30"/>
+      <c r="L64" s="29"/>
       <c r="M64" s="10"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -3376,13 +3407,13 @@
       <c r="D65" s="7"/>
       <c r="E65" s="6"/>
       <c r="F65" s="8"/>
-      <c r="H65" s="6">
+      <c r="H65" s="29">
         <v>11</v>
       </c>
-      <c r="I65" s="7"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="7"/>
-      <c r="L65" s="6"/>
+      <c r="I65" s="30"/>
+      <c r="J65" s="29"/>
+      <c r="K65" s="30"/>
+      <c r="L65" s="29"/>
       <c r="M65" s="10"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -3394,13 +3425,13 @@
       <c r="D66" s="7"/>
       <c r="E66" s="6"/>
       <c r="F66" s="8"/>
-      <c r="H66" s="6">
-        <v>12</v>
-      </c>
-      <c r="I66" s="7"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="7"/>
-      <c r="L66" s="6"/>
+      <c r="H66" s="29">
+        <v>12</v>
+      </c>
+      <c r="I66" s="30"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="30"/>
+      <c r="L66" s="29"/>
       <c r="M66" s="10"/>
       <c r="P66" s="1"/>
     </row>
@@ -3428,52 +3459,52 @@
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E74" s="2"/>
       <c r="F74" s="8"/>
-      <c r="L74" s="2"/>
+      <c r="L74" s="35"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E75" s="2"/>
       <c r="F75" s="8"/>
-      <c r="L75" s="2"/>
+      <c r="L75" s="35"/>
     </row>
     <row r="76" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A76" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="A76" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
       <c r="F76" s="8"/>
-      <c r="H76" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="18"/>
+      <c r="H76" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I76" s="25"/>
+      <c r="J76" s="25"/>
+      <c r="K76" s="25"/>
+      <c r="L76" s="25"/>
+      <c r="M76" s="12"/>
     </row>
     <row r="77" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
+      <c r="A77" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="12"/>
-      <c r="C77" s="13" t="s">
+      <c r="B77" s="22"/>
+      <c r="C77" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
       <c r="F77" s="8"/>
-      <c r="H77" s="12" t="s">
+      <c r="H77" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I77" s="12"/>
+      <c r="I77" s="26"/>
       <c r="J77" s="27" t="s">
         <v>39</v>
       </c>
       <c r="K77" s="27"/>
       <c r="L77" s="27"/>
-      <c r="M77" s="19"/>
+      <c r="M77" s="13"/>
     </row>
     <row r="78" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
@@ -3492,22 +3523,22 @@
         <v>5</v>
       </c>
       <c r="F78" s="8"/>
-      <c r="H78" s="5" t="s">
+      <c r="H78" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I78" s="5" t="s">
+      <c r="I78" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J78" s="5" t="s">
+      <c r="J78" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K78" s="5" t="s">
+      <c r="K78" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L78" s="5" t="s">
+      <c r="L78" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M78" s="20"/>
+      <c r="M78" s="14"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
@@ -3528,23 +3559,23 @@
       <c r="F79" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G79" s="17"/>
-      <c r="H79" s="6">
+      <c r="G79" s="11"/>
+      <c r="H79" s="29">
         <v>1</v>
       </c>
-      <c r="I79" s="7" t="s">
+      <c r="I79" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="J79" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K79" s="7" t="s">
+      <c r="J79" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K79" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="L79" s="6">
+      <c r="L79" s="29">
         <v>7989703873</v>
       </c>
-      <c r="M79" s="26"/>
+      <c r="M79" s="20"/>
       <c r="N79" s="6"/>
       <c r="O79" s="7"/>
       <c r="P79" s="6"/>
@@ -3568,23 +3599,23 @@
       <c r="F80" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G80" s="17"/>
-      <c r="H80" s="6">
+      <c r="G80" s="11"/>
+      <c r="H80" s="29">
         <v>2</v>
       </c>
-      <c r="I80" s="7" t="s">
+      <c r="I80" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="J80" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K80" s="7" t="s">
+      <c r="J80" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K80" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="L80" s="6">
+      <c r="L80" s="29">
         <v>8500903721</v>
       </c>
-      <c r="M80" s="26" t="s">
+      <c r="M80" s="20" t="s">
         <v>81</v>
       </c>
       <c r="N80" s="6" t="s">
@@ -3593,7 +3624,7 @@
       <c r="O80" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="P80" s="21">
+      <c r="P80" s="15">
         <v>9494325757</v>
       </c>
     </row>
@@ -3616,23 +3647,23 @@
       <c r="F81" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G81" s="17"/>
-      <c r="H81" s="6">
+      <c r="G81" s="11"/>
+      <c r="H81" s="29">
         <v>3</v>
       </c>
-      <c r="I81" s="7" t="s">
+      <c r="I81" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="J81" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K81" s="7" t="s">
+      <c r="J81" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K81" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="L81" s="6">
+      <c r="L81" s="29">
         <v>9492746481</v>
       </c>
-      <c r="M81" s="26" t="s">
+      <c r="M81" s="20" t="s">
         <v>85</v>
       </c>
       <c r="N81" s="6" t="s">
@@ -3641,7 +3672,7 @@
       <c r="O81" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="P81" s="21">
+      <c r="P81" s="15">
         <v>9492589395</v>
       </c>
       <c r="R81" s="1"/>
@@ -3665,20 +3696,20 @@
       <c r="F82" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G82" s="17"/>
-      <c r="H82" s="6">
+      <c r="G82" s="11"/>
+      <c r="H82" s="29">
         <v>4</v>
       </c>
-      <c r="I82" s="7" t="s">
+      <c r="I82" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="J82" s="6" t="s">
+      <c r="J82" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="K82" s="7" t="s">
+      <c r="K82" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="L82" s="6">
+      <c r="L82" s="29">
         <v>9491572320</v>
       </c>
     </row>
@@ -3701,20 +3732,20 @@
       <c r="F83" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G83" s="17"/>
-      <c r="H83" s="6">
+      <c r="G83" s="11"/>
+      <c r="H83" s="29">
         <v>5</v>
       </c>
-      <c r="I83" s="7" t="s">
+      <c r="I83" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="J83" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K83" s="7" t="s">
+      <c r="J83" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K83" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="L83" s="6">
+      <c r="L83" s="29">
         <v>8985385303</v>
       </c>
     </row>
@@ -3737,20 +3768,20 @@
       <c r="F84" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G84" s="17"/>
-      <c r="H84" s="6">
+      <c r="G84" s="11"/>
+      <c r="H84" s="29">
         <v>6</v>
       </c>
-      <c r="I84" s="7" t="s">
+      <c r="I84" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="J84" s="6" t="s">
+      <c r="J84" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="K84" s="7" t="s">
+      <c r="K84" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="L84" s="6">
+      <c r="L84" s="29">
         <v>7816039906</v>
       </c>
     </row>
@@ -3763,13 +3794,13 @@
       <c r="D85" s="7"/>
       <c r="E85" s="6"/>
       <c r="F85" s="8"/>
-      <c r="H85" s="6">
+      <c r="H85" s="29">
         <v>7</v>
       </c>
-      <c r="I85" s="28"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="28"/>
-      <c r="L85" s="29"/>
+      <c r="I85" s="36"/>
+      <c r="J85" s="37"/>
+      <c r="K85" s="36"/>
+      <c r="L85" s="37"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
@@ -3780,13 +3811,13 @@
       <c r="D86" s="7"/>
       <c r="E86" s="6"/>
       <c r="F86" s="8"/>
-      <c r="H86" s="6">
+      <c r="H86" s="29">
         <v>8</v>
       </c>
-      <c r="I86" s="7"/>
-      <c r="J86" s="6"/>
-      <c r="K86" s="7"/>
-      <c r="L86" s="6"/>
+      <c r="I86" s="30"/>
+      <c r="J86" s="29"/>
+      <c r="K86" s="30"/>
+      <c r="L86" s="29"/>
       <c r="M86" s="10"/>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
@@ -3798,13 +3829,13 @@
       <c r="D87" s="7"/>
       <c r="E87" s="6"/>
       <c r="F87" s="8"/>
-      <c r="H87" s="6">
+      <c r="H87" s="29">
         <v>9</v>
       </c>
-      <c r="I87" s="7"/>
-      <c r="J87" s="6"/>
-      <c r="K87" s="7"/>
-      <c r="L87" s="6"/>
+      <c r="I87" s="30"/>
+      <c r="J87" s="29"/>
+      <c r="K87" s="30"/>
+      <c r="L87" s="29"/>
       <c r="M87" s="10"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
@@ -3816,13 +3847,13 @@
       <c r="D88" s="7"/>
       <c r="E88" s="6"/>
       <c r="F88" s="8"/>
-      <c r="H88" s="6">
+      <c r="H88" s="29">
         <v>10</v>
       </c>
-      <c r="I88" s="7"/>
-      <c r="J88" s="6"/>
-      <c r="K88" s="7"/>
-      <c r="L88" s="6"/>
+      <c r="I88" s="30"/>
+      <c r="J88" s="29"/>
+      <c r="K88" s="30"/>
+      <c r="L88" s="29"/>
       <c r="M88" s="10"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
@@ -3834,13 +3865,13 @@
       <c r="D89" s="7"/>
       <c r="E89" s="6"/>
       <c r="F89" s="8"/>
-      <c r="H89" s="6">
+      <c r="H89" s="29">
         <v>11</v>
       </c>
-      <c r="I89" s="7"/>
-      <c r="J89" s="6"/>
-      <c r="K89" s="7"/>
-      <c r="L89" s="6"/>
+      <c r="I89" s="30"/>
+      <c r="J89" s="29"/>
+      <c r="K89" s="30"/>
+      <c r="L89" s="29"/>
       <c r="M89" s="10"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
@@ -3852,13 +3883,13 @@
       <c r="D90" s="7"/>
       <c r="E90" s="6"/>
       <c r="F90" s="8"/>
-      <c r="H90" s="6">
-        <v>12</v>
-      </c>
-      <c r="I90" s="7"/>
-      <c r="J90" s="6"/>
-      <c r="K90" s="7"/>
-      <c r="L90" s="6"/>
+      <c r="H90" s="29">
+        <v>12</v>
+      </c>
+      <c r="I90" s="30"/>
+      <c r="J90" s="29"/>
+      <c r="K90" s="30"/>
+      <c r="L90" s="29"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F91" s="8"/>
@@ -3897,44 +3928,44 @@
       <c r="F102" s="8"/>
     </row>
     <row r="103" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A103" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
+      <c r="A103" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
       <c r="F103" s="8"/>
-      <c r="H103" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
-      <c r="L103" s="11"/>
-      <c r="M103" s="18"/>
+      <c r="H103" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I103" s="25"/>
+      <c r="J103" s="25"/>
+      <c r="K103" s="25"/>
+      <c r="L103" s="25"/>
+      <c r="M103" s="12"/>
     </row>
     <row r="104" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
+      <c r="A104" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B104" s="12"/>
-      <c r="C104" s="13" t="s">
+      <c r="B104" s="22"/>
+      <c r="C104" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D104" s="14"/>
-      <c r="E104" s="14"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
       <c r="F104" s="8"/>
-      <c r="H104" s="12" t="s">
+      <c r="H104" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I104" s="12"/>
+      <c r="I104" s="26"/>
       <c r="J104" s="27" t="s">
         <v>76</v>
       </c>
       <c r="K104" s="27"/>
       <c r="L104" s="27"/>
-      <c r="M104" s="19"/>
+      <c r="M104" s="13"/>
     </row>
     <row r="105" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
@@ -3953,22 +3984,22 @@
         <v>5</v>
       </c>
       <c r="F105" s="8"/>
-      <c r="H105" s="5" t="s">
+      <c r="H105" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="I105" s="5" t="s">
+      <c r="I105" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J105" s="5" t="s">
+      <c r="J105" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K105" s="5" t="s">
+      <c r="K105" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L105" s="5" t="s">
+      <c r="L105" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="M105" s="20"/>
+      <c r="M105" s="14"/>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
@@ -3989,24 +4020,24 @@
       <c r="F106" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G106" s="17"/>
-      <c r="H106" s="6">
+      <c r="G106" s="11"/>
+      <c r="H106" s="29">
         <v>1</v>
       </c>
-      <c r="I106" s="7" t="s">
+      <c r="I106" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J106" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K106" s="7" t="s">
+      <c r="J106" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K106" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="L106" s="6">
+      <c r="L106" s="29">
         <v>9494771725</v>
       </c>
       <c r="M106" s="10"/>
-      <c r="N106" s="25"/>
+      <c r="N106" s="19"/>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="6">
@@ -4027,24 +4058,24 @@
       <c r="F107" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G107" s="17"/>
-      <c r="H107" s="6">
+      <c r="G107" s="11"/>
+      <c r="H107" s="29">
         <v>2</v>
       </c>
-      <c r="I107" s="7" t="s">
+      <c r="I107" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="J107" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K107" s="7" t="s">
+      <c r="J107" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K107" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="L107" s="6">
+      <c r="L107" s="29">
         <v>9121083391</v>
       </c>
       <c r="M107" s="10"/>
-      <c r="N107" s="25"/>
+      <c r="N107" s="19"/>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="6">
@@ -4065,24 +4096,24 @@
       <c r="F108" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G108" s="17"/>
-      <c r="H108" s="6">
+      <c r="G108" s="11"/>
+      <c r="H108" s="29">
         <v>3</v>
       </c>
-      <c r="I108" s="7" t="s">
+      <c r="I108" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="J108" s="6" t="s">
+      <c r="J108" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="K108" s="7" t="s">
+      <c r="K108" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="L108" s="6">
+      <c r="L108" s="29">
         <v>9494779528</v>
       </c>
       <c r="M108" s="10"/>
-      <c r="N108" s="25"/>
+      <c r="N108" s="19"/>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
@@ -4103,23 +4134,23 @@
       <c r="F109" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G109" s="17"/>
-      <c r="H109" s="6">
+      <c r="G109" s="11"/>
+      <c r="H109" s="29">
         <v>4</v>
       </c>
       <c r="I109" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="J109" s="29" t="s">
+      <c r="J109" s="37" t="s">
         <v>9</v>
       </c>
       <c r="K109" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="L109" s="29">
+      <c r="L109" s="37">
         <v>9553705650</v>
       </c>
-      <c r="M109" s="26" t="s">
+      <c r="M109" s="20" t="s">
         <v>82</v>
       </c>
       <c r="N109" s="6" t="s">
@@ -4151,24 +4182,24 @@
       <c r="F110" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G110" s="17"/>
-      <c r="H110" s="6">
+      <c r="G110" s="11"/>
+      <c r="H110" s="29">
         <v>5</v>
       </c>
-      <c r="I110" s="7" t="s">
+      <c r="I110" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="J110" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K110" s="7" t="s">
+      <c r="J110" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K110" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="L110" s="6">
+      <c r="L110" s="29">
         <v>8500955318</v>
       </c>
       <c r="M110" s="10"/>
-      <c r="N110" s="25"/>
+      <c r="N110" s="19"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="6">
@@ -4189,24 +4220,24 @@
       <c r="F111" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="G111" s="17"/>
-      <c r="H111" s="6">
+      <c r="G111" s="11"/>
+      <c r="H111" s="29">
         <v>6</v>
       </c>
-      <c r="I111" s="7" t="s">
+      <c r="I111" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="J111" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K111" s="7" t="s">
+      <c r="J111" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K111" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="L111" s="6">
+      <c r="L111" s="29">
         <v>9182349589</v>
       </c>
       <c r="M111" s="10"/>
-      <c r="N111" s="25"/>
+      <c r="N111" s="19"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
@@ -4227,19 +4258,19 @@
       <c r="F112" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H112" s="6">
+      <c r="H112" s="29">
         <v>7</v>
       </c>
-      <c r="I112" s="7" t="s">
+      <c r="I112" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="J112" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K112" s="7" t="s">
+      <c r="J112" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K112" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="L112" s="6">
+      <c r="L112" s="29">
         <v>9493238068</v>
       </c>
     </row>
@@ -4262,19 +4293,19 @@
       <c r="F113" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H113" s="6">
+      <c r="H113" s="29">
         <v>8</v>
       </c>
-      <c r="I113" s="7" t="s">
+      <c r="I113" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="J113" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K113" s="7" t="s">
+      <c r="J113" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K113" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="L113" s="6">
+      <c r="L113" s="29">
         <v>9963606866</v>
       </c>
     </row>
@@ -4297,20 +4328,20 @@
       <c r="F114" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H114" s="6">
+      <c r="H114" s="29">
         <v>9</v>
       </c>
-      <c r="I114" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J114" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K114" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L114" s="6">
-        <v>9494779417</v>
+      <c r="I114" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="J114" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K114" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="L114" s="29">
+        <v>6305961181</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -4322,13 +4353,13 @@
       <c r="D115" s="7"/>
       <c r="E115" s="6"/>
       <c r="F115" s="8"/>
-      <c r="H115" s="6">
+      <c r="H115" s="29">
         <v>10</v>
       </c>
-      <c r="I115" s="7"/>
-      <c r="J115" s="6"/>
-      <c r="K115" s="7"/>
-      <c r="L115" s="6"/>
+      <c r="I115" s="30"/>
+      <c r="J115" s="29"/>
+      <c r="K115" s="30"/>
+      <c r="L115" s="29"/>
       <c r="M115" s="10"/>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -4340,13 +4371,13 @@
       <c r="D116" s="7"/>
       <c r="E116" s="6"/>
       <c r="F116" s="8"/>
-      <c r="H116" s="6">
+      <c r="H116" s="29">
         <v>11</v>
       </c>
-      <c r="I116" s="7"/>
-      <c r="J116" s="6"/>
-      <c r="K116" s="7"/>
-      <c r="L116" s="6"/>
+      <c r="I116" s="30"/>
+      <c r="J116" s="29"/>
+      <c r="K116" s="30"/>
+      <c r="L116" s="29"/>
       <c r="M116" s="10"/>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -4358,13 +4389,13 @@
       <c r="D117" s="7"/>
       <c r="E117" s="6"/>
       <c r="F117" s="8"/>
-      <c r="H117" s="6">
-        <v>12</v>
-      </c>
-      <c r="I117" s="7"/>
-      <c r="J117" s="6"/>
-      <c r="K117" s="7"/>
-      <c r="L117" s="6"/>
+      <c r="H117" s="29">
+        <v>12</v>
+      </c>
+      <c r="I117" s="30"/>
+      <c r="J117" s="29"/>
+      <c r="K117" s="30"/>
+      <c r="L117" s="29"/>
       <c r="M117" s="10"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -4682,36 +4713,36 @@
     <sortCondition ref="V4:V146"/>
   </sortState>
   <mergeCells count="30">
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="H26:L26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="H52:L52"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="J53:L53"/>
     <mergeCell ref="H76:L76"/>
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="J77:L77"/>
     <mergeCell ref="H103:L103"/>
     <mergeCell ref="H104:I104"/>
     <mergeCell ref="J104:L104"/>
-    <mergeCell ref="H26:L26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="H52:L52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J53:L53"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="A76:E76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:E77"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.33" bottom="0.37" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>